<commit_message>
Added project files for pico FreeRTOS
</commit_message>
<xml_diff>
--- a/documentation/design-process/gantt-chart.xlsx
+++ b/documentation/design-process/gantt-chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b704535d3b4bef12/Documents/a University/Fifth Year/capstone-project/documentation/design-process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{8BC0CED1-54EB-44EA-A1E2-266196A5F329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3A7BDF3-CDEF-4141-A85D-4538F47E9B7B}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{8BC0CED1-54EB-44EA-A1E2-266196A5F329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FFE0338-EB2E-4654-99C0-CBDE3B8BBB4E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -571,11 +571,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -630,6 +667,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -657,12 +695,6 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -675,7 +707,13 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,7 +940,7 @@
   <dimension ref="A1:AH999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+      <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -917,54 +955,54 @@
       <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="49" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="49" t="s">
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="49" t="s">
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="49" t="s">
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="49" t="s">
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="49" t="s">
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="50"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="49" t="s">
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="47"/>
-      <c r="AH1" s="48"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="68"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="31">
@@ -986,11 +1024,11 @@
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="52" t="s">
+      <c r="P2" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="55" t="s">
+      <c r="Q2" s="54"/>
+      <c r="R2" s="56" t="s">
         <v>29</v>
       </c>
       <c r="S2" s="4"/>
@@ -999,7 +1037,7 @@
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
       <c r="X2" s="4"/>
-      <c r="Y2" s="10"/>
+      <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
@@ -1007,10 +1045,10 @@
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
-      <c r="AG2" s="59" t="s">
+      <c r="AG2" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="60"/>
+      <c r="AH2" s="61"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="31">
@@ -1032,16 +1070,16 @@
       <c r="M3" s="16"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="53"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="56"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="57"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
-      <c r="Y3" s="10"/>
+      <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
@@ -1049,8 +1087,8 @@
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
-      <c r="AG3" s="61"/>
-      <c r="AH3" s="62"/>
+      <c r="AG3" s="60"/>
+      <c r="AH3" s="61"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="31"/>
@@ -1070,16 +1108,16 @@
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="56"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="57"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
       <c r="X4" s="4"/>
-      <c r="Y4" s="10"/>
+      <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
@@ -1087,8 +1125,8 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
-      <c r="AG4" s="61"/>
-      <c r="AH4" s="62"/>
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="61"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="31">
@@ -1110,16 +1148,16 @@
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="56"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="57"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
       <c r="X5" s="4"/>
-      <c r="Y5" s="10"/>
+      <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
@@ -1127,8 +1165,8 @@
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
-      <c r="AG5" s="61"/>
-      <c r="AH5" s="62"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="61"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="31">
@@ -1150,16 +1188,16 @@
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="53"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="56"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="57"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
-      <c r="Y6" s="10"/>
+      <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
@@ -1167,8 +1205,8 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
-      <c r="AG6" s="61"/>
-      <c r="AH6" s="62"/>
+      <c r="AG6" s="60"/>
+      <c r="AH6" s="61"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="31">
@@ -1190,16 +1228,16 @@
       <c r="M7" s="18"/>
       <c r="N7" s="20"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="56"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="57"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
-      <c r="Y7" s="10"/>
+      <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
@@ -1207,8 +1245,8 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
-      <c r="AG7" s="61"/>
-      <c r="AH7" s="62"/>
+      <c r="AG7" s="60"/>
+      <c r="AH7" s="61"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="31">
@@ -1230,16 +1268,16 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="56"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="57"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
-      <c r="Y8" s="10"/>
+      <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
@@ -1247,8 +1285,8 @@
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
-      <c r="AG8" s="61"/>
-      <c r="AH8" s="62"/>
+      <c r="AG8" s="60"/>
+      <c r="AH8" s="61"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="31"/>
@@ -1268,16 +1306,16 @@
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
       <c r="O9" s="18"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="56"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="57"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
-      <c r="Y9" s="10"/>
+      <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
@@ -1285,8 +1323,8 @@
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
-      <c r="AG9" s="61"/>
-      <c r="AH9" s="62"/>
+      <c r="AG9" s="60"/>
+      <c r="AH9" s="61"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="31">
@@ -1308,16 +1346,16 @@
       <c r="M10" s="15"/>
       <c r="N10" s="42"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="56"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="57"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="10"/>
+      <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
@@ -1325,8 +1363,8 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
-      <c r="AG10" s="61"/>
-      <c r="AH10" s="62"/>
+      <c r="AG10" s="60"/>
+      <c r="AH10" s="61"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="31">
@@ -1348,16 +1386,16 @@
       <c r="M11" s="18"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="56"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="57"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="10"/>
+      <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
@@ -1365,8 +1403,8 @@
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
-      <c r="AG11" s="61"/>
-      <c r="AH11" s="62"/>
+      <c r="AG11" s="60"/>
+      <c r="AH11" s="61"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="31">
@@ -1388,16 +1426,16 @@
       <c r="M12" s="17"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="56"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="57"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="10"/>
+      <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
@@ -1405,8 +1443,8 @@
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
-      <c r="AG12" s="61"/>
-      <c r="AH12" s="62"/>
+      <c r="AG12" s="60"/>
+      <c r="AH12" s="61"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="31">
@@ -1428,16 +1466,16 @@
       <c r="M13" s="16"/>
       <c r="N13" s="43"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="53"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="56"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="57"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
-      <c r="Y13" s="10"/>
+      <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
@@ -1445,8 +1483,8 @@
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
-      <c r="AG13" s="61"/>
-      <c r="AH13" s="62"/>
+      <c r="AG13" s="60"/>
+      <c r="AH13" s="61"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="31">
@@ -1468,9 +1506,9 @@
       <c r="M14" s="22"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
-      <c r="P14" s="53"/>
-      <c r="Q14" s="53"/>
-      <c r="R14" s="56"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="57"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -1485,8 +1523,8 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
-      <c r="AG14" s="61"/>
-      <c r="AH14" s="62"/>
+      <c r="AG14" s="60"/>
+      <c r="AH14" s="61"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="31">
@@ -1508,9 +1546,9 @@
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
-      <c r="P15" s="53"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="57"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="58"/>
       <c r="S15" s="44"/>
       <c r="T15" s="44"/>
       <c r="U15" s="44"/>
@@ -1525,8 +1563,8 @@
       <c r="AD15" s="44"/>
       <c r="AE15" s="44"/>
       <c r="AF15" s="44"/>
-      <c r="AG15" s="61"/>
-      <c r="AH15" s="62"/>
+      <c r="AG15" s="60"/>
+      <c r="AH15" s="61"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="31">
@@ -1548,14 +1586,14 @@
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="12"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="57"/>
+      <c r="P16" s="55"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="58"/>
       <c r="S16" s="24"/>
       <c r="T16" s="24"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
-      <c r="W16" s="30"/>
+      <c r="U16" s="64"/>
+      <c r="V16" s="64"/>
+      <c r="W16" s="29"/>
       <c r="X16" s="29"/>
       <c r="Y16" s="17"/>
       <c r="Z16" s="16"/>
@@ -1565,8 +1603,8 @@
       <c r="AD16" s="16"/>
       <c r="AE16" s="16"/>
       <c r="AF16" s="16"/>
-      <c r="AG16" s="61"/>
-      <c r="AH16" s="62"/>
+      <c r="AG16" s="60"/>
+      <c r="AH16" s="61"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A17" s="31">
@@ -1588,9 +1626,9 @@
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="57"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="58"/>
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
       <c r="U17" s="29"/>
@@ -1605,8 +1643,8 @@
       <c r="AD17" s="16"/>
       <c r="AE17" s="16"/>
       <c r="AF17" s="16"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="62"/>
+      <c r="AG17" s="60"/>
+      <c r="AH17" s="61"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A18" s="31">
@@ -1628,9 +1666,9 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="57"/>
+      <c r="P18" s="55"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="58"/>
       <c r="S18" s="18"/>
       <c r="T18" s="21"/>
       <c r="U18" s="21"/>
@@ -1645,8 +1683,8 @@
       <c r="AD18" s="16"/>
       <c r="AE18" s="16"/>
       <c r="AF18" s="16"/>
-      <c r="AG18" s="61"/>
-      <c r="AH18" s="62"/>
+      <c r="AG18" s="60"/>
+      <c r="AH18" s="61"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A19" s="31">
@@ -1668,14 +1706,14 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="57"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="58"/>
       <c r="S19" s="18"/>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
-      <c r="V19" s="65"/>
-      <c r="W19" s="65"/>
+      <c r="V19" s="46"/>
+      <c r="W19" s="46"/>
       <c r="X19" s="20"/>
       <c r="Y19" s="23"/>
       <c r="Z19" s="20"/>
@@ -1685,8 +1723,8 @@
       <c r="AD19" s="16"/>
       <c r="AE19" s="16"/>
       <c r="AF19" s="16"/>
-      <c r="AG19" s="61"/>
-      <c r="AH19" s="62"/>
+      <c r="AG19" s="60"/>
+      <c r="AH19" s="61"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A20" s="31">
@@ -1708,9 +1746,9 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="14"/>
-      <c r="P20" s="54"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="57"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="58"/>
       <c r="S20" s="23"/>
       <c r="T20" s="23"/>
       <c r="U20" s="21"/>
@@ -1725,8 +1763,8 @@
       <c r="AD20" s="16"/>
       <c r="AE20" s="16"/>
       <c r="AF20" s="16"/>
-      <c r="AG20" s="61"/>
-      <c r="AH20" s="62"/>
+      <c r="AG20" s="60"/>
+      <c r="AH20" s="61"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A21" s="31">
@@ -1748,9 +1786,9 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="14"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="57"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="58"/>
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
       <c r="U21" s="18"/>
@@ -1765,8 +1803,8 @@
       <c r="AD21" s="16"/>
       <c r="AE21" s="16"/>
       <c r="AF21" s="16"/>
-      <c r="AG21" s="61"/>
-      <c r="AH21" s="62"/>
+      <c r="AG21" s="60"/>
+      <c r="AH21" s="61"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A22" s="31">
@@ -1788,9 +1826,9 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="13"/>
-      <c r="P22" s="54"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="57"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="58"/>
       <c r="S22" s="18"/>
       <c r="T22" s="18"/>
       <c r="U22" s="18"/>
@@ -1805,8 +1843,8 @@
       <c r="AD22" s="16"/>
       <c r="AE22" s="16"/>
       <c r="AF22" s="16"/>
-      <c r="AG22" s="61"/>
-      <c r="AH22" s="62"/>
+      <c r="AG22" s="60"/>
+      <c r="AH22" s="61"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A23" s="31">
@@ -1828,9 +1866,9 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="13"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="53"/>
-      <c r="R23" s="57"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="58"/>
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
       <c r="U23" s="18"/>
@@ -1845,8 +1883,8 @@
       <c r="AD23" s="16"/>
       <c r="AE23" s="16"/>
       <c r="AF23" s="16"/>
-      <c r="AG23" s="61"/>
-      <c r="AH23" s="62"/>
+      <c r="AG23" s="60"/>
+      <c r="AH23" s="61"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A24" s="31">
@@ -1868,14 +1906,14 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="14"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="57"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="58"/>
       <c r="S24" s="18"/>
       <c r="T24" s="18"/>
       <c r="U24" s="18"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="19"/>
       <c r="X24" s="20"/>
       <c r="Y24" s="23"/>
       <c r="Z24" s="20"/>
@@ -1885,8 +1923,8 @@
       <c r="AD24" s="20"/>
       <c r="AE24" s="16"/>
       <c r="AF24" s="16"/>
-      <c r="AG24" s="61"/>
-      <c r="AH24" s="62"/>
+      <c r="AG24" s="60"/>
+      <c r="AH24" s="61"/>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A25" s="31">
@@ -1908,9 +1946,9 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="13"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="57"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="58"/>
       <c r="S25" s="20"/>
       <c r="T25" s="20"/>
       <c r="U25" s="20"/>
@@ -1925,8 +1963,8 @@
       <c r="AD25" s="20"/>
       <c r="AE25" s="16"/>
       <c r="AF25" s="16"/>
-      <c r="AG25" s="61"/>
-      <c r="AH25" s="62"/>
+      <c r="AG25" s="60"/>
+      <c r="AH25" s="61"/>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A26" s="31">
@@ -1948,9 +1986,9 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="14"/>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="57"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="58"/>
       <c r="S26" s="18"/>
       <c r="T26" s="18"/>
       <c r="U26" s="18"/>
@@ -1965,8 +2003,8 @@
       <c r="AD26" s="20"/>
       <c r="AE26" s="16"/>
       <c r="AF26" s="16"/>
-      <c r="AG26" s="61"/>
-      <c r="AH26" s="62"/>
+      <c r="AG26" s="60"/>
+      <c r="AH26" s="61"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A27" s="31">
@@ -1988,9 +2026,9 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="14"/>
-      <c r="P27" s="54"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="57"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="58"/>
       <c r="S27" s="18"/>
       <c r="T27" s="18"/>
       <c r="U27" s="18"/>
@@ -2005,8 +2043,8 @@
       <c r="AD27" s="20"/>
       <c r="AE27" s="16"/>
       <c r="AF27" s="16"/>
-      <c r="AG27" s="61"/>
-      <c r="AH27" s="62"/>
+      <c r="AG27" s="60"/>
+      <c r="AH27" s="61"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A28" s="31">
@@ -2028,9 +2066,9 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="54"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="57"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="58"/>
       <c r="S28" s="20"/>
       <c r="T28" s="20"/>
       <c r="U28" s="20"/>
@@ -2045,8 +2083,8 @@
       <c r="AD28" s="20"/>
       <c r="AE28" s="16"/>
       <c r="AF28" s="16"/>
-      <c r="AG28" s="61"/>
-      <c r="AH28" s="62"/>
+      <c r="AG28" s="60"/>
+      <c r="AH28" s="61"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A29" s="31">
@@ -2068,9 +2106,9 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="54"/>
-      <c r="Q29" s="53"/>
-      <c r="R29" s="57"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="58"/>
       <c r="S29" s="20"/>
       <c r="T29" s="20"/>
       <c r="U29" s="20"/>
@@ -2085,8 +2123,8 @@
       <c r="AD29" s="20"/>
       <c r="AE29" s="16"/>
       <c r="AF29" s="16"/>
-      <c r="AG29" s="61"/>
-      <c r="AH29" s="62"/>
+      <c r="AG29" s="60"/>
+      <c r="AH29" s="61"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A30" s="31">
@@ -2108,9 +2146,9 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="53"/>
-      <c r="R30" s="57"/>
+      <c r="P30" s="55"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="58"/>
       <c r="S30" s="16"/>
       <c r="T30" s="16"/>
       <c r="U30" s="16"/>
@@ -2125,8 +2163,8 @@
       <c r="AD30" s="20"/>
       <c r="AE30" s="16"/>
       <c r="AF30" s="16"/>
-      <c r="AG30" s="61"/>
-      <c r="AH30" s="62"/>
+      <c r="AG30" s="60"/>
+      <c r="AH30" s="61"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A31" s="31">
@@ -2148,9 +2186,9 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="54"/>
-      <c r="Q31" s="53"/>
-      <c r="R31" s="57"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="58"/>
       <c r="S31" s="16"/>
       <c r="T31" s="16"/>
       <c r="U31" s="16"/>
@@ -2165,8 +2203,8 @@
       <c r="AD31" s="20"/>
       <c r="AE31" s="16"/>
       <c r="AF31" s="16"/>
-      <c r="AG31" s="61"/>
-      <c r="AH31" s="62"/>
+      <c r="AG31" s="60"/>
+      <c r="AH31" s="61"/>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B32" s="37" t="s">
@@ -2185,9 +2223,9 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-      <c r="P32" s="54"/>
-      <c r="Q32" s="53"/>
-      <c r="R32" s="57"/>
+      <c r="P32" s="55"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="58"/>
       <c r="S32" s="16"/>
       <c r="T32" s="16"/>
       <c r="U32" s="16"/>
@@ -2202,8 +2240,8 @@
       <c r="AD32" s="26"/>
       <c r="AE32" s="26"/>
       <c r="AF32" s="16"/>
-      <c r="AG32" s="61"/>
-      <c r="AH32" s="62"/>
+      <c r="AG32" s="60"/>
+      <c r="AH32" s="61"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B33" s="37" t="s">
@@ -2222,9 +2260,9 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="54"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="57"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="58"/>
       <c r="S33" s="16"/>
       <c r="T33" s="16"/>
       <c r="U33" s="16"/>
@@ -2239,8 +2277,8 @@
       <c r="AD33" s="18"/>
       <c r="AE33" s="26"/>
       <c r="AF33" s="26"/>
-      <c r="AG33" s="61"/>
-      <c r="AH33" s="62"/>
+      <c r="AG33" s="60"/>
+      <c r="AH33" s="61"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B34" s="37" t="s">
@@ -2259,9 +2297,9 @@
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="54"/>
-      <c r="Q34" s="53"/>
-      <c r="R34" s="57"/>
+      <c r="P34" s="55"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="58"/>
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
       <c r="U34" s="16"/>
@@ -2276,8 +2314,8 @@
       <c r="AD34" s="16"/>
       <c r="AE34" s="18"/>
       <c r="AF34" s="16"/>
-      <c r="AG34" s="61"/>
-      <c r="AH34" s="62"/>
+      <c r="AG34" s="60"/>
+      <c r="AH34" s="61"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B35" s="16" t="s">
@@ -2296,9 +2334,9 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="54"/>
-      <c r="Q35" s="53"/>
-      <c r="R35" s="57"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="58"/>
       <c r="S35" s="39"/>
       <c r="T35" s="39"/>
       <c r="U35" s="39"/>
@@ -2313,8 +2351,8 @@
       <c r="AD35" s="41"/>
       <c r="AE35" s="41"/>
       <c r="AF35" s="20"/>
-      <c r="AG35" s="61"/>
-      <c r="AH35" s="62"/>
+      <c r="AG35" s="60"/>
+      <c r="AH35" s="61"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A36" s="31"/>
@@ -2332,9 +2370,9 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="58"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="59"/>
       <c r="S36" s="16"/>
       <c r="T36" s="16"/>
       <c r="U36" s="16"/>
@@ -2349,8 +2387,8 @@
       <c r="AD36" s="16"/>
       <c r="AE36" s="16"/>
       <c r="AF36" s="16"/>
-      <c r="AG36" s="63"/>
-      <c r="AH36" s="64"/>
+      <c r="AG36" s="62"/>
+      <c r="AH36" s="63"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:34" x14ac:dyDescent="0.2"/>
@@ -2359,117 +2397,117 @@
     <row r="41" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="47"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="47"/>
-      <c r="M42" s="47"/>
-      <c r="N42" s="47"/>
-      <c r="O42" s="47"/>
-      <c r="P42" s="47"/>
-      <c r="Q42" s="47"/>
-      <c r="R42" s="47"/>
-      <c r="S42" s="47"/>
-      <c r="T42" s="47"/>
-      <c r="U42" s="47"/>
-      <c r="V42" s="47"/>
-      <c r="W42" s="47"/>
-      <c r="X42" s="47"/>
-      <c r="Y42" s="47"/>
-      <c r="Z42" s="47"/>
-      <c r="AA42" s="47"/>
-      <c r="AB42" s="47"/>
-      <c r="AC42" s="47"/>
-      <c r="AD42" s="47"/>
-      <c r="AE42" s="47"/>
-      <c r="AF42" s="47"/>
-      <c r="AG42" s="47"/>
-      <c r="AH42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="48"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="48"/>
+      <c r="O42" s="48"/>
+      <c r="P42" s="48"/>
+      <c r="Q42" s="48"/>
+      <c r="R42" s="48"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
+      <c r="U42" s="48"/>
+      <c r="V42" s="48"/>
+      <c r="W42" s="48"/>
+      <c r="X42" s="48"/>
+      <c r="Y42" s="48"/>
+      <c r="Z42" s="48"/>
+      <c r="AA42" s="48"/>
+      <c r="AB42" s="48"/>
+      <c r="AC42" s="48"/>
+      <c r="AD42" s="48"/>
+      <c r="AE42" s="48"/>
+      <c r="AF42" s="48"/>
+      <c r="AG42" s="48"/>
+      <c r="AH42" s="49"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
-      <c r="B43" s="46" t="s">
+      <c r="B43" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="47"/>
-      <c r="N43" s="47"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="47"/>
-      <c r="Q43" s="47"/>
-      <c r="R43" s="47"/>
-      <c r="S43" s="47"/>
-      <c r="T43" s="47"/>
-      <c r="U43" s="47"/>
-      <c r="V43" s="47"/>
-      <c r="W43" s="47"/>
-      <c r="X43" s="47"/>
-      <c r="Y43" s="47"/>
-      <c r="Z43" s="47"/>
-      <c r="AA43" s="47"/>
-      <c r="AB43" s="47"/>
-      <c r="AC43" s="47"/>
-      <c r="AD43" s="47"/>
-      <c r="AE43" s="47"/>
-      <c r="AF43" s="47"/>
-      <c r="AG43" s="47"/>
-      <c r="AH43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="48"/>
+      <c r="U43" s="48"/>
+      <c r="V43" s="48"/>
+      <c r="W43" s="48"/>
+      <c r="X43" s="48"/>
+      <c r="Y43" s="48"/>
+      <c r="Z43" s="48"/>
+      <c r="AA43" s="48"/>
+      <c r="AB43" s="48"/>
+      <c r="AC43" s="48"/>
+      <c r="AD43" s="48"/>
+      <c r="AE43" s="48"/>
+      <c r="AF43" s="48"/>
+      <c r="AG43" s="48"/>
+      <c r="AH43" s="49"/>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="47"/>
-      <c r="M44" s="47"/>
-      <c r="N44" s="47"/>
-      <c r="O44" s="47"/>
-      <c r="P44" s="47"/>
-      <c r="Q44" s="47"/>
-      <c r="R44" s="47"/>
-      <c r="S44" s="47"/>
-      <c r="T44" s="47"/>
-      <c r="U44" s="47"/>
-      <c r="V44" s="47"/>
-      <c r="W44" s="47"/>
-      <c r="X44" s="47"/>
-      <c r="Y44" s="47"/>
-      <c r="Z44" s="47"/>
-      <c r="AA44" s="47"/>
-      <c r="AB44" s="47"/>
-      <c r="AC44" s="47"/>
-      <c r="AD44" s="47"/>
-      <c r="AE44" s="47"/>
-      <c r="AF44" s="47"/>
-      <c r="AG44" s="47"/>
-      <c r="AH44" s="48"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="48"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="48"/>
+      <c r="P44" s="48"/>
+      <c r="Q44" s="48"/>
+      <c r="R44" s="48"/>
+      <c r="S44" s="48"/>
+      <c r="T44" s="48"/>
+      <c r="U44" s="48"/>
+      <c r="V44" s="48"/>
+      <c r="W44" s="48"/>
+      <c r="X44" s="48"/>
+      <c r="Y44" s="48"/>
+      <c r="Z44" s="48"/>
+      <c r="AA44" s="48"/>
+      <c r="AB44" s="48"/>
+      <c r="AC44" s="48"/>
+      <c r="AD44" s="48"/>
+      <c r="AE44" s="48"/>
+      <c r="AF44" s="48"/>
+      <c r="AG44" s="48"/>
+      <c r="AH44" s="49"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
@@ -2511,41 +2549,41 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="47"/>
-      <c r="M46" s="47"/>
-      <c r="N46" s="47"/>
-      <c r="O46" s="47"/>
-      <c r="P46" s="47"/>
-      <c r="Q46" s="47"/>
-      <c r="R46" s="47"/>
-      <c r="S46" s="47"/>
-      <c r="T46" s="47"/>
-      <c r="U46" s="47"/>
-      <c r="V46" s="47"/>
-      <c r="W46" s="47"/>
-      <c r="X46" s="47"/>
-      <c r="Y46" s="47"/>
-      <c r="Z46" s="47"/>
-      <c r="AA46" s="47"/>
-      <c r="AB46" s="47"/>
-      <c r="AC46" s="47"/>
-      <c r="AD46" s="47"/>
-      <c r="AE46" s="47"/>
-      <c r="AF46" s="47"/>
-      <c r="AG46" s="47"/>
-      <c r="AH46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="48"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="48"/>
+      <c r="S46" s="48"/>
+      <c r="T46" s="48"/>
+      <c r="U46" s="48"/>
+      <c r="V46" s="48"/>
+      <c r="W46" s="48"/>
+      <c r="X46" s="48"/>
+      <c r="Y46" s="48"/>
+      <c r="Z46" s="48"/>
+      <c r="AA46" s="48"/>
+      <c r="AB46" s="48"/>
+      <c r="AC46" s="48"/>
+      <c r="AD46" s="48"/>
+      <c r="AE46" s="48"/>
+      <c r="AF46" s="48"/>
+      <c r="AG46" s="48"/>
+      <c r="AH46" s="49"/>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>

</xml_diff>

<commit_message>
Added ability to read from firebase database and get updates from database
</commit_message>
<xml_diff>
--- a/documentation/design-process/gantt-chart.xlsx
+++ b/documentation/design-process/gantt-chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b704535d3b4bef12/Documents/a University/Fifth Year/capstone-project/documentation/design-process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{8BC0CED1-54EB-44EA-A1E2-266196A5F329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FFE0338-EB2E-4654-99C0-CBDE3B8BBB4E}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{8BC0CED1-54EB-44EA-A1E2-266196A5F329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1AFAAFC-D1B4-478C-B0B2-63CDE4FDCE00}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -249,8 +249,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +370,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -612,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -647,7 +660,6 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -666,14 +678,17 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -695,10 +710,13 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -707,13 +725,14 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,10 +748,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -940,7 +955,7 @@
   <dimension ref="A1:AH999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+      <selection activeCell="Z30" sqref="Z30:AC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -952,66 +967,66 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="50" t="s">
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="50" t="s">
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="50" t="s">
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="66" t="s">
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="66" t="s">
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="66" t="s">
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="66" t="s">
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="68"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="54"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A2" s="31">
+      <c r="A2" s="30">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="16"/>
@@ -1024,11 +1039,11 @@
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="53" t="s">
+      <c r="P2" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="56" t="s">
+      <c r="Q2" s="56"/>
+      <c r="R2" s="58" t="s">
         <v>29</v>
       </c>
       <c r="S2" s="4"/>
@@ -1045,19 +1060,19 @@
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
-      <c r="AG2" s="65" t="s">
+      <c r="AG2" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="61"/>
+      <c r="AH2" s="63"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="31">
+      <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="15"/>
@@ -1070,9 +1085,9 @@
       <c r="M3" s="16"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="57"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="59"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
@@ -1087,15 +1102,15 @@
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
-      <c r="AG3" s="60"/>
-      <c r="AH3" s="61"/>
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="63"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
@@ -1108,9 +1123,9 @@
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="57"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="59"/>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -1125,17 +1140,17 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="61"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="63"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A5" s="31">
+      <c r="A5" s="30">
         <v>3</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="34"/>
+      <c r="C5" s="33"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -1148,9 +1163,9 @@
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="57"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="59"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
@@ -1165,17 +1180,17 @@
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
-      <c r="AG5" s="60"/>
-      <c r="AH5" s="61"/>
+      <c r="AG5" s="64"/>
+      <c r="AH5" s="63"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A6" s="31">
+      <c r="A6" s="30">
         <v>4</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="34"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -1188,9 +1203,9 @@
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="57"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="59"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
@@ -1205,17 +1220,17 @@
       <c r="AD6" s="4"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
-      <c r="AG6" s="60"/>
-      <c r="AH6" s="61"/>
+      <c r="AG6" s="64"/>
+      <c r="AH6" s="63"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="31">
+      <c r="A7" s="30">
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -1228,9 +1243,9 @@
       <c r="M7" s="18"/>
       <c r="N7" s="20"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="57"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="59"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -1245,17 +1260,17 @@
       <c r="AD7" s="4"/>
       <c r="AE7" s="4"/>
       <c r="AF7" s="4"/>
-      <c r="AG7" s="60"/>
-      <c r="AH7" s="61"/>
+      <c r="AG7" s="64"/>
+      <c r="AH7" s="63"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="31">
+      <c r="A8" s="30">
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -1268,9 +1283,9 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="57"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="59"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
@@ -1285,15 +1300,15 @@
       <c r="AD8" s="4"/>
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
-      <c r="AG8" s="60"/>
-      <c r="AH8" s="61"/>
+      <c r="AG8" s="64"/>
+      <c r="AH8" s="63"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="33"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -1306,9 +1321,9 @@
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
       <c r="O9" s="18"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="57"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="59"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -1323,17 +1338,17 @@
       <c r="AD9" s="4"/>
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
-      <c r="AG9" s="60"/>
-      <c r="AH9" s="61"/>
+      <c r="AG9" s="64"/>
+      <c r="AH9" s="63"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" s="31">
+      <c r="A10" s="30">
         <v>7</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -1344,11 +1359,11 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="42"/>
+      <c r="N10" s="41"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="57"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="59"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
@@ -1363,17 +1378,17 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="4"/>
-      <c r="AG10" s="60"/>
-      <c r="AH10" s="61"/>
+      <c r="AG10" s="64"/>
+      <c r="AH10" s="63"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" s="31">
+      <c r="A11" s="30">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="33"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -1386,9 +1401,9 @@
       <c r="M11" s="18"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="57"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="59"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -1403,17 +1418,17 @@
       <c r="AD11" s="4"/>
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
-      <c r="AG11" s="60"/>
-      <c r="AH11" s="61"/>
+      <c r="AG11" s="64"/>
+      <c r="AH11" s="63"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="31">
+      <c r="A12" s="30">
         <v>9</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -1426,9 +1441,9 @@
       <c r="M12" s="17"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="57"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="59"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
@@ -1443,17 +1458,17 @@
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
-      <c r="AG12" s="60"/>
-      <c r="AH12" s="61"/>
+      <c r="AG12" s="64"/>
+      <c r="AH12" s="63"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="31">
+      <c r="A13" s="30">
         <v>10</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -1464,11 +1479,11 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
-      <c r="N13" s="43"/>
+      <c r="N13" s="42"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="57"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="59"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
@@ -1483,17 +1498,17 @@
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
-      <c r="AG13" s="60"/>
-      <c r="AH13" s="61"/>
+      <c r="AG13" s="64"/>
+      <c r="AH13" s="63"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A14" s="31">
+      <c r="A14" s="30">
         <v>11</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
@@ -1506,9 +1521,9 @@
       <c r="M14" s="22"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="57"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="59"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -1523,17 +1538,17 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
       <c r="AF14" s="4"/>
-      <c r="AG14" s="60"/>
-      <c r="AH14" s="61"/>
+      <c r="AG14" s="64"/>
+      <c r="AH14" s="63"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A15" s="31">
+      <c r="A15" s="30">
         <v>12</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="15"/>
@@ -1546,31 +1561,31 @@
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="58"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="44"/>
-      <c r="AA15" s="44"/>
-      <c r="AB15" s="44"/>
-      <c r="AC15" s="44"/>
-      <c r="AD15" s="44"/>
-      <c r="AE15" s="44"/>
-      <c r="AF15" s="44"/>
-      <c r="AG15" s="60"/>
-      <c r="AH15" s="61"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="67"/>
+      <c r="T15" s="67"/>
+      <c r="U15" s="67"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="67"/>
+      <c r="X15" s="67"/>
+      <c r="Y15" s="68"/>
+      <c r="Z15" s="67"/>
+      <c r="AA15" s="43"/>
+      <c r="AB15" s="43"/>
+      <c r="AC15" s="43"/>
+      <c r="AD15" s="43"/>
+      <c r="AE15" s="43"/>
+      <c r="AF15" s="43"/>
+      <c r="AG15" s="64"/>
+      <c r="AH15" s="63"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A16" s="31">
+      <c r="A16" s="30">
         <v>13</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="36" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="10"/>
@@ -1586,13 +1601,13 @@
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="12"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="58"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="60"/>
       <c r="S16" s="24"/>
       <c r="T16" s="24"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="64"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
       <c r="W16" s="29"/>
       <c r="X16" s="29"/>
       <c r="Y16" s="17"/>
@@ -1603,14 +1618,14 @@
       <c r="AD16" s="16"/>
       <c r="AE16" s="16"/>
       <c r="AF16" s="16"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="61"/>
+      <c r="AG16" s="64"/>
+      <c r="AH16" s="63"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A17" s="31">
+      <c r="A17" s="30">
         <v>14</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="4"/>
@@ -1626,16 +1641,16 @@
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="58"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="60"/>
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
       <c r="U17" s="29"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="29"/>
-      <c r="Y17" s="17"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="72"/>
       <c r="Z17" s="16"/>
       <c r="AA17" s="16"/>
       <c r="AB17" s="16"/>
@@ -1643,14 +1658,14 @@
       <c r="AD17" s="16"/>
       <c r="AE17" s="16"/>
       <c r="AF17" s="16"/>
-      <c r="AG17" s="60"/>
-      <c r="AH17" s="61"/>
+      <c r="AG17" s="64"/>
+      <c r="AH17" s="63"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A18" s="31">
+      <c r="A18" s="30">
         <v>15</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="4"/>
@@ -1666,16 +1681,16 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="58"/>
+      <c r="P18" s="57"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="60"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="28"/>
-      <c r="W18" s="28"/>
-      <c r="X18" s="20"/>
-      <c r="Y18" s="23"/>
+      <c r="T18" s="69"/>
+      <c r="U18" s="69"/>
+      <c r="V18" s="70"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="72"/>
       <c r="Z18" s="20"/>
       <c r="AA18" s="16"/>
       <c r="AB18" s="16"/>
@@ -1683,14 +1698,14 @@
       <c r="AD18" s="16"/>
       <c r="AE18" s="16"/>
       <c r="AF18" s="16"/>
-      <c r="AG18" s="60"/>
-      <c r="AH18" s="61"/>
+      <c r="AG18" s="64"/>
+      <c r="AH18" s="63"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A19" s="31">
+      <c r="A19" s="30">
         <v>16</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="4"/>
@@ -1706,14 +1721,14 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="58"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="60"/>
       <c r="S19" s="18"/>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="46"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="44"/>
       <c r="X19" s="20"/>
       <c r="Y19" s="23"/>
       <c r="Z19" s="20"/>
@@ -1723,14 +1738,14 @@
       <c r="AD19" s="16"/>
       <c r="AE19" s="16"/>
       <c r="AF19" s="16"/>
-      <c r="AG19" s="60"/>
-      <c r="AH19" s="61"/>
+      <c r="AG19" s="64"/>
+      <c r="AH19" s="63"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A20" s="31">
+      <c r="A20" s="30">
         <v>17</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="36" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="4"/>
@@ -1746,31 +1761,31 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="14"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="58"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="60"/>
       <c r="S20" s="23"/>
       <c r="T20" s="23"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="20"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="71"/>
+      <c r="W20" s="71"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="73"/>
+      <c r="Z20" s="28"/>
       <c r="AA20" s="16"/>
       <c r="AB20" s="16"/>
       <c r="AC20" s="16"/>
       <c r="AD20" s="16"/>
       <c r="AE20" s="16"/>
       <c r="AF20" s="16"/>
-      <c r="AG20" s="60"/>
-      <c r="AH20" s="61"/>
+      <c r="AG20" s="64"/>
+      <c r="AH20" s="63"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A21" s="31">
+      <c r="A21" s="30">
         <v>18</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="4"/>
@@ -1786,28 +1801,28 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="14"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="58"/>
+      <c r="P21" s="57"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="60"/>
       <c r="S21" s="23"/>
       <c r="T21" s="23"/>
       <c r="U21" s="18"/>
       <c r="V21" s="18"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="20"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="20"/>
+      <c r="W21" s="28"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="73"/>
+      <c r="Z21" s="28"/>
       <c r="AA21" s="16"/>
       <c r="AB21" s="16"/>
       <c r="AC21" s="16"/>
       <c r="AD21" s="16"/>
       <c r="AE21" s="16"/>
       <c r="AF21" s="16"/>
-      <c r="AG21" s="60"/>
-      <c r="AH21" s="61"/>
+      <c r="AG21" s="64"/>
+      <c r="AH21" s="63"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A22" s="31">
+      <c r="A22" s="30">
         <v>19</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1826,16 +1841,16 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="13"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="54"/>
-      <c r="R22" s="58"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="60"/>
       <c r="S22" s="18"/>
       <c r="T22" s="18"/>
       <c r="U22" s="18"/>
       <c r="V22" s="16"/>
       <c r="W22" s="16"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="27"/>
+      <c r="X22" s="19"/>
+      <c r="Y22" s="72"/>
       <c r="Z22" s="16"/>
       <c r="AA22" s="16"/>
       <c r="AB22" s="16"/>
@@ -1843,11 +1858,11 @@
       <c r="AD22" s="16"/>
       <c r="AE22" s="16"/>
       <c r="AF22" s="16"/>
-      <c r="AG22" s="60"/>
-      <c r="AH22" s="61"/>
+      <c r="AG22" s="64"/>
+      <c r="AH22" s="63"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A23" s="31">
+      <c r="A23" s="30">
         <v>20</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -1866,9 +1881,9 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="13"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="58"/>
+      <c r="P23" s="57"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="60"/>
       <c r="S23" s="18"/>
       <c r="T23" s="18"/>
       <c r="U23" s="18"/>
@@ -1883,14 +1898,14 @@
       <c r="AD23" s="16"/>
       <c r="AE23" s="16"/>
       <c r="AF23" s="16"/>
-      <c r="AG23" s="60"/>
-      <c r="AH23" s="61"/>
+      <c r="AG23" s="64"/>
+      <c r="AH23" s="63"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A24" s="31">
+      <c r="A24" s="30">
         <v>21</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>38</v>
       </c>
       <c r="C24" s="4"/>
@@ -1906,9 +1921,9 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="14"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="58"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="60"/>
       <c r="S24" s="18"/>
       <c r="T24" s="18"/>
       <c r="U24" s="18"/>
@@ -1923,14 +1938,14 @@
       <c r="AD24" s="20"/>
       <c r="AE24" s="16"/>
       <c r="AF24" s="16"/>
-      <c r="AG24" s="60"/>
-      <c r="AH24" s="61"/>
+      <c r="AG24" s="64"/>
+      <c r="AH24" s="63"/>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A25" s="31">
+      <c r="A25" s="30">
         <v>22</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="4"/>
@@ -1946,14 +1961,14 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="13"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="58"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="60"/>
       <c r="S25" s="20"/>
       <c r="T25" s="20"/>
       <c r="U25" s="20"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="25"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="15"/>
       <c r="X25" s="18"/>
       <c r="Y25" s="23"/>
       <c r="Z25" s="20"/>
@@ -1963,14 +1978,14 @@
       <c r="AD25" s="20"/>
       <c r="AE25" s="16"/>
       <c r="AF25" s="16"/>
-      <c r="AG25" s="60"/>
-      <c r="AH25" s="61"/>
+      <c r="AG25" s="64"/>
+      <c r="AH25" s="63"/>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A26" s="31">
+      <c r="A26" s="30">
         <v>23</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="4"/>
@@ -1986,14 +2001,14 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="14"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="58"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="60"/>
       <c r="S26" s="18"/>
       <c r="T26" s="18"/>
       <c r="U26" s="18"/>
-      <c r="V26" s="25"/>
-      <c r="W26" s="26"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="19"/>
       <c r="X26" s="20"/>
       <c r="Y26" s="23"/>
       <c r="Z26" s="20"/>
@@ -2003,14 +2018,14 @@
       <c r="AD26" s="20"/>
       <c r="AE26" s="16"/>
       <c r="AF26" s="16"/>
-      <c r="AG26" s="60"/>
-      <c r="AH26" s="61"/>
+      <c r="AG26" s="64"/>
+      <c r="AH26" s="63"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A27" s="31">
+      <c r="A27" s="30">
         <v>24</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="36" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="4"/>
@@ -2026,31 +2041,31 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="14"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="58"/>
+      <c r="P27" s="57"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="60"/>
       <c r="S27" s="18"/>
       <c r="T27" s="18"/>
       <c r="U27" s="18"/>
-      <c r="V27" s="25"/>
-      <c r="W27" s="26"/>
-      <c r="X27" s="20"/>
-      <c r="Y27" s="23"/>
-      <c r="Z27" s="20"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="28"/>
+      <c r="X27" s="28"/>
+      <c r="Y27" s="73"/>
+      <c r="Z27" s="28"/>
       <c r="AA27" s="20"/>
       <c r="AB27" s="20"/>
       <c r="AC27" s="20"/>
       <c r="AD27" s="20"/>
       <c r="AE27" s="16"/>
       <c r="AF27" s="16"/>
-      <c r="AG27" s="60"/>
-      <c r="AH27" s="61"/>
+      <c r="AG27" s="64"/>
+      <c r="AH27" s="63"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A28" s="31">
+      <c r="A28" s="30">
         <v>25</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="4"/>
@@ -2066,14 +2081,14 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="58"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="60"/>
       <c r="S28" s="20"/>
       <c r="T28" s="20"/>
       <c r="U28" s="20"/>
-      <c r="V28" s="26"/>
-      <c r="W28" s="26"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
       <c r="X28" s="20"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
@@ -2083,14 +2098,14 @@
       <c r="AD28" s="20"/>
       <c r="AE28" s="16"/>
       <c r="AF28" s="16"/>
-      <c r="AG28" s="60"/>
-      <c r="AH28" s="61"/>
+      <c r="AG28" s="64"/>
+      <c r="AH28" s="63"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A29" s="31">
+      <c r="A29" s="30">
         <v>26</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="36" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="4"/>
@@ -2106,28 +2121,28 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="58"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="60"/>
       <c r="S29" s="20"/>
       <c r="T29" s="20"/>
       <c r="U29" s="20"/>
       <c r="V29" s="20"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="18"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="21"/>
+      <c r="Z29" s="21"/>
       <c r="AA29" s="23"/>
       <c r="AB29" s="20"/>
       <c r="AC29" s="20"/>
       <c r="AD29" s="20"/>
       <c r="AE29" s="16"/>
       <c r="AF29" s="16"/>
-      <c r="AG29" s="60"/>
-      <c r="AH29" s="61"/>
+      <c r="AG29" s="64"/>
+      <c r="AH29" s="63"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A30" s="31">
+      <c r="A30" s="30">
         <v>27</v>
       </c>
       <c r="B30" s="16" t="s">
@@ -2146,9 +2161,9 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="58"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="60"/>
       <c r="S30" s="16"/>
       <c r="T30" s="16"/>
       <c r="U30" s="16"/>
@@ -2163,14 +2178,14 @@
       <c r="AD30" s="20"/>
       <c r="AE30" s="16"/>
       <c r="AF30" s="16"/>
-      <c r="AG30" s="60"/>
-      <c r="AH30" s="61"/>
+      <c r="AG30" s="64"/>
+      <c r="AH30" s="63"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A31" s="31">
+      <c r="A31" s="30">
         <v>28</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="36" t="s">
         <v>46</v>
       </c>
       <c r="C31" s="4"/>
@@ -2186,9 +2201,9 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="58"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="60"/>
       <c r="S31" s="16"/>
       <c r="T31" s="16"/>
       <c r="U31" s="16"/>
@@ -2203,11 +2218,11 @@
       <c r="AD31" s="20"/>
       <c r="AE31" s="16"/>
       <c r="AF31" s="16"/>
-      <c r="AG31" s="60"/>
-      <c r="AH31" s="61"/>
+      <c r="AG31" s="64"/>
+      <c r="AH31" s="63"/>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="36" t="s">
         <v>47</v>
       </c>
       <c r="C32" s="4"/>
@@ -2223,9 +2238,9 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="54"/>
-      <c r="R32" s="58"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="56"/>
+      <c r="R32" s="60"/>
       <c r="S32" s="16"/>
       <c r="T32" s="16"/>
       <c r="U32" s="16"/>
@@ -2240,11 +2255,11 @@
       <c r="AD32" s="26"/>
       <c r="AE32" s="26"/>
       <c r="AF32" s="16"/>
-      <c r="AG32" s="60"/>
-      <c r="AH32" s="61"/>
+      <c r="AG32" s="64"/>
+      <c r="AH32" s="63"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="4"/>
@@ -2260,9 +2275,9 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="54"/>
-      <c r="R33" s="58"/>
+      <c r="P33" s="57"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="60"/>
       <c r="S33" s="16"/>
       <c r="T33" s="16"/>
       <c r="U33" s="16"/>
@@ -2277,11 +2292,11 @@
       <c r="AD33" s="18"/>
       <c r="AE33" s="26"/>
       <c r="AF33" s="26"/>
-      <c r="AG33" s="60"/>
-      <c r="AH33" s="61"/>
+      <c r="AG33" s="64"/>
+      <c r="AH33" s="63"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="36" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="4"/>
@@ -2297,9 +2312,9 @@
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="54"/>
-      <c r="R34" s="58"/>
+      <c r="P34" s="57"/>
+      <c r="Q34" s="56"/>
+      <c r="R34" s="60"/>
       <c r="S34" s="16"/>
       <c r="T34" s="16"/>
       <c r="U34" s="16"/>
@@ -2314,8 +2329,8 @@
       <c r="AD34" s="16"/>
       <c r="AE34" s="18"/>
       <c r="AF34" s="16"/>
-      <c r="AG34" s="60"/>
-      <c r="AH34" s="61"/>
+      <c r="AG34" s="64"/>
+      <c r="AH34" s="63"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B35" s="16" t="s">
@@ -2334,28 +2349,28 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="54"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="39"/>
-      <c r="T35" s="39"/>
-      <c r="U35" s="39"/>
-      <c r="V35" s="39"/>
-      <c r="W35" s="39"/>
-      <c r="X35" s="39"/>
-      <c r="Y35" s="40"/>
-      <c r="Z35" s="39"/>
-      <c r="AA35" s="41"/>
-      <c r="AB35" s="41"/>
-      <c r="AC35" s="41"/>
-      <c r="AD35" s="41"/>
-      <c r="AE35" s="41"/>
+      <c r="P35" s="57"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="38"/>
+      <c r="T35" s="38"/>
+      <c r="U35" s="38"/>
+      <c r="V35" s="38"/>
+      <c r="W35" s="38"/>
+      <c r="X35" s="38"/>
+      <c r="Y35" s="39"/>
+      <c r="Z35" s="38"/>
+      <c r="AA35" s="40"/>
+      <c r="AB35" s="40"/>
+      <c r="AC35" s="40"/>
+      <c r="AD35" s="40"/>
+      <c r="AE35" s="40"/>
       <c r="AF35" s="20"/>
-      <c r="AG35" s="60"/>
-      <c r="AH35" s="61"/>
+      <c r="AG35" s="64"/>
+      <c r="AH35" s="63"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A36" s="31"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="16"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -2370,9 +2385,9 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="59"/>
+      <c r="P36" s="57"/>
+      <c r="Q36" s="56"/>
+      <c r="R36" s="61"/>
       <c r="S36" s="16"/>
       <c r="T36" s="16"/>
       <c r="U36" s="16"/>
@@ -2387,8 +2402,8 @@
       <c r="AD36" s="16"/>
       <c r="AE36" s="16"/>
       <c r="AF36" s="16"/>
-      <c r="AG36" s="62"/>
-      <c r="AH36" s="63"/>
+      <c r="AG36" s="65"/>
+      <c r="AH36" s="66"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:34" x14ac:dyDescent="0.2"/>
@@ -2397,117 +2412,117 @@
     <row r="41" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="48"/>
-      <c r="O42" s="48"/>
-      <c r="P42" s="48"/>
-      <c r="Q42" s="48"/>
-      <c r="R42" s="48"/>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
-      <c r="U42" s="48"/>
-      <c r="V42" s="48"/>
-      <c r="W42" s="48"/>
-      <c r="X42" s="48"/>
-      <c r="Y42" s="48"/>
-      <c r="Z42" s="48"/>
-      <c r="AA42" s="48"/>
-      <c r="AB42" s="48"/>
-      <c r="AC42" s="48"/>
-      <c r="AD42" s="48"/>
-      <c r="AE42" s="48"/>
-      <c r="AF42" s="48"/>
-      <c r="AG42" s="48"/>
-      <c r="AH42" s="49"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="47"/>
+      <c r="S42" s="47"/>
+      <c r="T42" s="47"/>
+      <c r="U42" s="47"/>
+      <c r="V42" s="47"/>
+      <c r="W42" s="47"/>
+      <c r="X42" s="47"/>
+      <c r="Y42" s="47"/>
+      <c r="Z42" s="47"/>
+      <c r="AA42" s="47"/>
+      <c r="AB42" s="47"/>
+      <c r="AC42" s="47"/>
+      <c r="AD42" s="47"/>
+      <c r="AE42" s="47"/>
+      <c r="AF42" s="47"/>
+      <c r="AG42" s="47"/>
+      <c r="AH42" s="48"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A43" s="8"/>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="48"/>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
-      <c r="U43" s="48"/>
-      <c r="V43" s="48"/>
-      <c r="W43" s="48"/>
-      <c r="X43" s="48"/>
-      <c r="Y43" s="48"/>
-      <c r="Z43" s="48"/>
-      <c r="AA43" s="48"/>
-      <c r="AB43" s="48"/>
-      <c r="AC43" s="48"/>
-      <c r="AD43" s="48"/>
-      <c r="AE43" s="48"/>
-      <c r="AF43" s="48"/>
-      <c r="AG43" s="48"/>
-      <c r="AH43" s="49"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="47"/>
+      <c r="S43" s="47"/>
+      <c r="T43" s="47"/>
+      <c r="U43" s="47"/>
+      <c r="V43" s="47"/>
+      <c r="W43" s="47"/>
+      <c r="X43" s="47"/>
+      <c r="Y43" s="47"/>
+      <c r="Z43" s="47"/>
+      <c r="AA43" s="47"/>
+      <c r="AB43" s="47"/>
+      <c r="AC43" s="47"/>
+      <c r="AD43" s="47"/>
+      <c r="AE43" s="47"/>
+      <c r="AF43" s="47"/>
+      <c r="AG43" s="47"/>
+      <c r="AH43" s="48"/>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-      <c r="O44" s="48"/>
-      <c r="P44" s="48"/>
-      <c r="Q44" s="48"/>
-      <c r="R44" s="48"/>
-      <c r="S44" s="48"/>
-      <c r="T44" s="48"/>
-      <c r="U44" s="48"/>
-      <c r="V44" s="48"/>
-      <c r="W44" s="48"/>
-      <c r="X44" s="48"/>
-      <c r="Y44" s="48"/>
-      <c r="Z44" s="48"/>
-      <c r="AA44" s="48"/>
-      <c r="AB44" s="48"/>
-      <c r="AC44" s="48"/>
-      <c r="AD44" s="48"/>
-      <c r="AE44" s="48"/>
-      <c r="AF44" s="48"/>
-      <c r="AG44" s="48"/>
-      <c r="AH44" s="49"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="47"/>
+      <c r="O44" s="47"/>
+      <c r="P44" s="47"/>
+      <c r="Q44" s="47"/>
+      <c r="R44" s="47"/>
+      <c r="S44" s="47"/>
+      <c r="T44" s="47"/>
+      <c r="U44" s="47"/>
+      <c r="V44" s="47"/>
+      <c r="W44" s="47"/>
+      <c r="X44" s="47"/>
+      <c r="Y44" s="47"/>
+      <c r="Z44" s="47"/>
+      <c r="AA44" s="47"/>
+      <c r="AB44" s="47"/>
+      <c r="AC44" s="47"/>
+      <c r="AD44" s="47"/>
+      <c r="AE44" s="47"/>
+      <c r="AF44" s="47"/>
+      <c r="AG44" s="47"/>
+      <c r="AH44" s="48"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
@@ -2549,41 +2564,41 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
-      <c r="O46" s="48"/>
-      <c r="P46" s="48"/>
-      <c r="Q46" s="48"/>
-      <c r="R46" s="48"/>
-      <c r="S46" s="48"/>
-      <c r="T46" s="48"/>
-      <c r="U46" s="48"/>
-      <c r="V46" s="48"/>
-      <c r="W46" s="48"/>
-      <c r="X46" s="48"/>
-      <c r="Y46" s="48"/>
-      <c r="Z46" s="48"/>
-      <c r="AA46" s="48"/>
-      <c r="AB46" s="48"/>
-      <c r="AC46" s="48"/>
-      <c r="AD46" s="48"/>
-      <c r="AE46" s="48"/>
-      <c r="AF46" s="48"/>
-      <c r="AG46" s="48"/>
-      <c r="AH46" s="49"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="47"/>
+      <c r="O46" s="47"/>
+      <c r="P46" s="47"/>
+      <c r="Q46" s="47"/>
+      <c r="R46" s="47"/>
+      <c r="S46" s="47"/>
+      <c r="T46" s="47"/>
+      <c r="U46" s="47"/>
+      <c r="V46" s="47"/>
+      <c r="W46" s="47"/>
+      <c r="X46" s="47"/>
+      <c r="Y46" s="47"/>
+      <c r="Z46" s="47"/>
+      <c r="AA46" s="47"/>
+      <c r="AB46" s="47"/>
+      <c r="AC46" s="47"/>
+      <c r="AD46" s="47"/>
+      <c r="AE46" s="47"/>
+      <c r="AF46" s="47"/>
+      <c r="AG46" s="47"/>
+      <c r="AH46" s="48"/>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>

</xml_diff>

<commit_message>
Added project day presentation and updated gantt-chart
</commit_message>
<xml_diff>
--- a/documentation/design-process/gantt-chart.xlsx
+++ b/documentation/design-process/gantt-chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b704535d3b4bef12/Documents/a University/Fifth Year/capstone-project/documentation/design-process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{8BC0CED1-54EB-44EA-A1E2-266196A5F329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1AFAAFC-D1B4-478C-B0B2-63CDE4FDCE00}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{8BC0CED1-54EB-44EA-A1E2-266196A5F329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2FB5B50-C459-4C2B-8B20-4128F224EBE0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>Exams</t>
-  </si>
-  <si>
-    <t>Demo week</t>
   </si>
   <si>
     <t>Development of Communication module</t>
@@ -257,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,12 +277,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCC0000"/>
         <bgColor rgb="FFCC0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF38761D"/>
       </patternFill>
     </fill>
     <fill>
@@ -320,12 +311,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FF38761D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFF1C232"/>
       </patternFill>
@@ -345,30 +330,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -637,49 +598,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -689,50 +650,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,10 +905,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AH999"/>
+  <dimension ref="A1:AH998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z30" sqref="Z30:AC31"/>
+      <selection activeCell="AL22" sqref="AL22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -967,7 +920,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="49" t="s">
@@ -1020,13 +973,13 @@
       <c r="AH1" s="54"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A2" s="30">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="16"/>
@@ -1066,13 +1019,13 @@
       <c r="AH2" s="63"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="30">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="15"/>
@@ -1106,11 +1059,11 @@
       <c r="AH3" s="63"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="36" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
@@ -1144,13 +1097,13 @@
       <c r="AH4" s="63"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A5" s="30">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="33"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -1184,13 +1137,13 @@
       <c r="AH5" s="63"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A6" s="30">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
@@ -1224,13 +1177,13 @@
       <c r="AH6" s="63"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="30">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="33"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -1264,13 +1217,13 @@
       <c r="AH7" s="63"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="30">
+      <c r="A8" s="25">
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="33"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
@@ -1304,11 +1257,11 @@
       <c r="AH8" s="63"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="36" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -1342,13 +1295,13 @@
       <c r="AH9" s="63"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" s="30">
+      <c r="A10" s="25">
         <v>7</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -1359,7 +1312,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="41"/>
+      <c r="N10" s="36"/>
       <c r="O10" s="15"/>
       <c r="P10" s="56"/>
       <c r="Q10" s="56"/>
@@ -1382,13 +1335,13 @@
       <c r="AH10" s="63"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" s="30">
+      <c r="A11" s="25">
         <v>8</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="33"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
@@ -1422,13 +1375,13 @@
       <c r="AH11" s="63"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="30">
+      <c r="A12" s="25">
         <v>9</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
@@ -1462,13 +1415,13 @@
       <c r="AH12" s="63"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A13" s="30">
+      <c r="A13" s="25">
         <v>10</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -1479,7 +1432,7 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
-      <c r="N13" s="42"/>
+      <c r="N13" s="37"/>
       <c r="O13" s="15"/>
       <c r="P13" s="56"/>
       <c r="Q13" s="56"/>
@@ -1502,23 +1455,23 @@
       <c r="AH13" s="63"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A14" s="30">
+      <c r="A14" s="25">
         <v>11</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
       <c r="P14" s="56"/>
@@ -1542,13 +1495,13 @@
       <c r="AH14" s="63"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A15" s="30">
+      <c r="A15" s="25">
         <v>12</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="15"/>
@@ -1564,29 +1517,29 @@
       <c r="P15" s="56"/>
       <c r="Q15" s="56"/>
       <c r="R15" s="60"/>
-      <c r="S15" s="67"/>
-      <c r="T15" s="67"/>
-      <c r="U15" s="67"/>
-      <c r="V15" s="67"/>
-      <c r="W15" s="67"/>
-      <c r="X15" s="67"/>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="67"/>
-      <c r="AA15" s="43"/>
-      <c r="AB15" s="43"/>
-      <c r="AC15" s="43"/>
-      <c r="AD15" s="43"/>
-      <c r="AE15" s="43"/>
-      <c r="AF15" s="43"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="40"/>
+      <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="40"/>
+      <c r="AC15" s="40"/>
+      <c r="AD15" s="40"/>
+      <c r="AE15" s="40"/>
+      <c r="AF15" s="40"/>
       <c r="AG15" s="64"/>
       <c r="AH15" s="63"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A16" s="30">
+      <c r="A16" s="25">
         <v>13</v>
       </c>
-      <c r="B16" s="36" t="s">
-        <v>35</v>
+      <c r="B16" s="31" t="s">
+        <v>34</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1604,12 +1557,12 @@
       <c r="P16" s="57"/>
       <c r="Q16" s="56"/>
       <c r="R16" s="60"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="29"/>
-      <c r="X16" s="29"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
       <c r="Y16" s="17"/>
       <c r="Z16" s="16"/>
       <c r="AA16" s="16"/>
@@ -1622,11 +1575,11 @@
       <c r="AH16" s="63"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A17" s="30">
+      <c r="A17" s="25">
         <v>14</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>36</v>
+      <c r="B17" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1644,13 +1597,13 @@
       <c r="P17" s="57"/>
       <c r="Q17" s="56"/>
       <c r="R17" s="60"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="29"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="72"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="39"/>
+      <c r="W17" s="39"/>
+      <c r="X17" s="39"/>
+      <c r="Y17" s="44"/>
       <c r="Z17" s="16"/>
       <c r="AA17" s="16"/>
       <c r="AB17" s="16"/>
@@ -1662,11 +1615,11 @@
       <c r="AH17" s="63"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A18" s="30">
+      <c r="A18" s="25">
         <v>15</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>37</v>
+      <c r="B18" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1685,12 +1638,12 @@
       <c r="Q18" s="56"/>
       <c r="R18" s="60"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="70"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="43"/>
       <c r="W18" s="19"/>
       <c r="X18" s="19"/>
-      <c r="Y18" s="72"/>
+      <c r="Y18" s="44"/>
       <c r="Z18" s="20"/>
       <c r="AA18" s="16"/>
       <c r="AB18" s="16"/>
@@ -1702,11 +1655,11 @@
       <c r="AH18" s="63"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A19" s="30">
+      <c r="A19" s="25">
         <v>16</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>48</v>
+      <c r="B19" s="31" t="s">
+        <v>47</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1727,10 +1680,10 @@
       <c r="S19" s="18"/>
       <c r="T19" s="15"/>
       <c r="U19" s="15"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="44"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
       <c r="X19" s="20"/>
-      <c r="Y19" s="23"/>
+      <c r="Y19" s="22"/>
       <c r="Z19" s="20"/>
       <c r="AA19" s="16"/>
       <c r="AB19" s="16"/>
@@ -1742,11 +1695,11 @@
       <c r="AH19" s="63"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A20" s="30">
+      <c r="A20" s="25">
         <v>17</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>44</v>
+      <c r="B20" s="31" t="s">
+        <v>43</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1764,16 +1717,16 @@
       <c r="P20" s="57"/>
       <c r="Q20" s="56"/>
       <c r="R20" s="60"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="71"/>
-      <c r="W20" s="71"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="73"/>
-      <c r="Z20" s="28"/>
-      <c r="AA20" s="16"/>
-      <c r="AB20" s="16"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="44"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
       <c r="AC20" s="16"/>
       <c r="AD20" s="16"/>
       <c r="AE20" s="16"/>
@@ -1782,11 +1735,11 @@
       <c r="AH20" s="63"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A21" s="30">
+      <c r="A21" s="25">
         <v>18</v>
       </c>
-      <c r="B21" s="36" t="s">
-        <v>45</v>
+      <c r="B21" s="31" t="s">
+        <v>44</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1804,14 +1757,14 @@
       <c r="P21" s="57"/>
       <c r="Q21" s="56"/>
       <c r="R21" s="60"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
       <c r="U21" s="18"/>
       <c r="V21" s="18"/>
-      <c r="W21" s="28"/>
-      <c r="X21" s="28"/>
-      <c r="Y21" s="73"/>
-      <c r="Z21" s="28"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="44"/>
+      <c r="Z21" s="19"/>
       <c r="AA21" s="16"/>
       <c r="AB21" s="16"/>
       <c r="AC21" s="16"/>
@@ -1822,7 +1775,7 @@
       <c r="AH21" s="63"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A22" s="30">
+      <c r="A22" s="25">
         <v>19</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1850,7 +1803,7 @@
       <c r="V22" s="16"/>
       <c r="W22" s="16"/>
       <c r="X22" s="19"/>
-      <c r="Y22" s="72"/>
+      <c r="Y22" s="44"/>
       <c r="Z22" s="16"/>
       <c r="AA22" s="16"/>
       <c r="AB22" s="16"/>
@@ -1862,7 +1815,7 @@
       <c r="AH22" s="63"/>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A23" s="30">
+      <c r="A23" s="25">
         <v>20</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -1890,10 +1843,10 @@
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
       <c r="X23" s="16"/>
-      <c r="Y23" s="23"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="16"/>
+      <c r="Y23" s="22"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19"/>
       <c r="AC23" s="16"/>
       <c r="AD23" s="16"/>
       <c r="AE23" s="16"/>
@@ -1902,11 +1855,11 @@
       <c r="AH23" s="63"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A24" s="30">
+      <c r="A24" s="25">
         <v>21</v>
       </c>
-      <c r="B24" s="36" t="s">
-        <v>38</v>
+      <c r="B24" s="31" t="s">
+        <v>37</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1930,7 +1883,7 @@
       <c r="V24" s="15"/>
       <c r="W24" s="19"/>
       <c r="X24" s="20"/>
-      <c r="Y24" s="23"/>
+      <c r="Y24" s="22"/>
       <c r="Z24" s="20"/>
       <c r="AA24" s="20"/>
       <c r="AB24" s="20"/>
@@ -1942,11 +1895,11 @@
       <c r="AH24" s="63"/>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A25" s="30">
+      <c r="A25" s="25">
         <v>22</v>
       </c>
-      <c r="B25" s="36" t="s">
-        <v>39</v>
+      <c r="B25" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1970,7 +1923,7 @@
       <c r="V25" s="19"/>
       <c r="W25" s="15"/>
       <c r="X25" s="18"/>
-      <c r="Y25" s="23"/>
+      <c r="Y25" s="22"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20"/>
       <c r="AB25" s="20"/>
@@ -1982,11 +1935,11 @@
       <c r="AH25" s="63"/>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A26" s="30">
+      <c r="A26" s="25">
         <v>23</v>
       </c>
-      <c r="B26" s="36" t="s">
-        <v>40</v>
+      <c r="B26" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -2010,7 +1963,7 @@
       <c r="V26" s="15"/>
       <c r="W26" s="19"/>
       <c r="X26" s="20"/>
-      <c r="Y26" s="23"/>
+      <c r="Y26" s="22"/>
       <c r="Z26" s="20"/>
       <c r="AA26" s="20"/>
       <c r="AB26" s="20"/>
@@ -2022,11 +1975,11 @@
       <c r="AH26" s="63"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A27" s="30">
+      <c r="A27" s="25">
         <v>24</v>
       </c>
-      <c r="B27" s="36" t="s">
-        <v>49</v>
+      <c r="B27" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2047,12 +2000,12 @@
       <c r="S27" s="18"/>
       <c r="T27" s="18"/>
       <c r="U27" s="18"/>
-      <c r="V27" s="21"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="73"/>
-      <c r="Z27" s="28"/>
-      <c r="AA27" s="20"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="44"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
       <c r="AB27" s="20"/>
       <c r="AC27" s="20"/>
       <c r="AD27" s="20"/>
@@ -2062,11 +2015,11 @@
       <c r="AH27" s="63"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A28" s="30">
+      <c r="A28" s="25">
         <v>25</v>
       </c>
-      <c r="B28" s="36" t="s">
-        <v>41</v>
+      <c r="B28" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -2092,7 +2045,7 @@
       <c r="X28" s="20"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
-      <c r="AA28" s="23"/>
+      <c r="AA28" s="22"/>
       <c r="AB28" s="20"/>
       <c r="AC28" s="20"/>
       <c r="AD28" s="20"/>
@@ -2102,11 +2055,11 @@
       <c r="AH28" s="63"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A29" s="30">
+      <c r="A29" s="25">
         <v>26</v>
       </c>
-      <c r="B29" s="36" t="s">
-        <v>43</v>
+      <c r="B29" s="31" t="s">
+        <v>42</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -2128,12 +2081,12 @@
       <c r="T29" s="20"/>
       <c r="U29" s="20"/>
       <c r="V29" s="20"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="28"/>
-      <c r="Y29" s="21"/>
-      <c r="Z29" s="21"/>
-      <c r="AA29" s="23"/>
-      <c r="AB29" s="20"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="44"/>
+      <c r="AB29" s="19"/>
       <c r="AC29" s="20"/>
       <c r="AD29" s="20"/>
       <c r="AE29" s="16"/>
@@ -2142,7 +2095,7 @@
       <c r="AH29" s="63"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A30" s="30">
+      <c r="A30" s="25">
         <v>27</v>
       </c>
       <c r="B30" s="16" t="s">
@@ -2170,11 +2123,11 @@
       <c r="V30" s="16"/>
       <c r="W30" s="18"/>
       <c r="X30" s="18"/>
-      <c r="Y30" s="23"/>
-      <c r="Z30" s="27"/>
-      <c r="AA30" s="26"/>
-      <c r="AB30" s="26"/>
-      <c r="AC30" s="26"/>
+      <c r="Y30" s="22"/>
+      <c r="Z30" s="44"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="19"/>
+      <c r="AC30" s="19"/>
       <c r="AD30" s="20"/>
       <c r="AE30" s="16"/>
       <c r="AF30" s="16"/>
@@ -2182,11 +2135,11 @@
       <c r="AH30" s="63"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A31" s="30">
+      <c r="A31" s="25">
         <v>28</v>
       </c>
-      <c r="B31" s="36" t="s">
-        <v>46</v>
+      <c r="B31" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -2210,20 +2163,20 @@
       <c r="V31" s="16"/>
       <c r="W31" s="16"/>
       <c r="X31" s="16"/>
-      <c r="Y31" s="23"/>
+      <c r="Y31" s="22"/>
       <c r="Z31" s="20"/>
       <c r="AA31" s="18"/>
-      <c r="AB31" s="25"/>
-      <c r="AC31" s="25"/>
-      <c r="AD31" s="20"/>
+      <c r="AB31" s="15"/>
+      <c r="AC31" s="15"/>
+      <c r="AD31" s="19"/>
       <c r="AE31" s="16"/>
       <c r="AF31" s="16"/>
       <c r="AG31" s="64"/>
       <c r="AH31" s="63"/>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B32" s="36" t="s">
-        <v>47</v>
+      <c r="B32" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -2247,20 +2200,20 @@
       <c r="V32" s="16"/>
       <c r="W32" s="16"/>
       <c r="X32" s="16"/>
-      <c r="Y32" s="23"/>
+      <c r="Y32" s="22"/>
       <c r="Z32" s="20"/>
       <c r="AA32" s="18"/>
       <c r="AB32" s="18"/>
       <c r="AC32" s="18"/>
-      <c r="AD32" s="26"/>
-      <c r="AE32" s="26"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
       <c r="AF32" s="16"/>
       <c r="AG32" s="64"/>
       <c r="AH32" s="63"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B33" s="36" t="s">
-        <v>34</v>
+      <c r="B33" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2284,20 +2237,20 @@
       <c r="V33" s="16"/>
       <c r="W33" s="16"/>
       <c r="X33" s="16"/>
-      <c r="Y33" s="23"/>
-      <c r="Z33" s="20"/>
-      <c r="AA33" s="20"/>
-      <c r="AB33" s="20"/>
-      <c r="AC33" s="20"/>
-      <c r="AD33" s="18"/>
-      <c r="AE33" s="26"/>
-      <c r="AF33" s="26"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="16"/>
+      <c r="AC33" s="16"/>
+      <c r="AD33" s="16"/>
+      <c r="AE33" s="18"/>
+      <c r="AF33" s="16"/>
       <c r="AG33" s="64"/>
       <c r="AH33" s="63"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B34" s="36" t="s">
-        <v>42</v>
+      <c r="B34" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -2315,27 +2268,26 @@
       <c r="P34" s="57"/>
       <c r="Q34" s="56"/>
       <c r="R34" s="60"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="16"/>
-      <c r="X34" s="16"/>
-      <c r="Y34" s="17"/>
-      <c r="Z34" s="16"/>
-      <c r="AA34" s="16"/>
-      <c r="AB34" s="16"/>
-      <c r="AC34" s="16"/>
-      <c r="AD34" s="16"/>
-      <c r="AE34" s="18"/>
-      <c r="AF34" s="16"/>
+      <c r="S34" s="33"/>
+      <c r="T34" s="33"/>
+      <c r="U34" s="33"/>
+      <c r="V34" s="33"/>
+      <c r="W34" s="33"/>
+      <c r="X34" s="33"/>
+      <c r="Y34" s="34"/>
+      <c r="Z34" s="33"/>
+      <c r="AA34" s="35"/>
+      <c r="AB34" s="35"/>
+      <c r="AC34" s="35"/>
+      <c r="AD34" s="35"/>
+      <c r="AE34" s="36"/>
+      <c r="AF34" s="19"/>
       <c r="AG34" s="64"/>
       <c r="AH34" s="63"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="B35" s="16" t="s">
-        <v>22</v>
-      </c>
+      <c r="A35" s="25"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2351,69 +2303,71 @@
       <c r="O35" s="4"/>
       <c r="P35" s="57"/>
       <c r="Q35" s="56"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="38"/>
-      <c r="T35" s="38"/>
-      <c r="U35" s="38"/>
-      <c r="V35" s="38"/>
-      <c r="W35" s="38"/>
-      <c r="X35" s="38"/>
-      <c r="Y35" s="39"/>
-      <c r="Z35" s="38"/>
-      <c r="AA35" s="40"/>
-      <c r="AB35" s="40"/>
-      <c r="AC35" s="40"/>
-      <c r="AD35" s="40"/>
-      <c r="AE35" s="40"/>
-      <c r="AF35" s="20"/>
-      <c r="AG35" s="64"/>
-      <c r="AH35" s="63"/>
-    </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="61"/>
-      <c r="S36" s="16"/>
-      <c r="T36" s="16"/>
-      <c r="U36" s="16"/>
-      <c r="V36" s="16"/>
-      <c r="W36" s="16"/>
-      <c r="X36" s="16"/>
-      <c r="Y36" s="27"/>
-      <c r="Z36" s="26"/>
-      <c r="AA36" s="26"/>
-      <c r="AB36" s="26"/>
-      <c r="AC36" s="26"/>
-      <c r="AD36" s="16"/>
-      <c r="AE36" s="16"/>
-      <c r="AF36" s="16"/>
-      <c r="AG36" s="65"/>
-      <c r="AH36" s="66"/>
-    </row>
+      <c r="R35" s="61"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="16"/>
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="65"/>
+      <c r="AH35" s="66"/>
+    </row>
+    <row r="36" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:34" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:34" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A41" s="7"/>
+      <c r="B41" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="47"/>
+      <c r="Q41" s="47"/>
+      <c r="R41" s="47"/>
+      <c r="S41" s="47"/>
+      <c r="T41" s="47"/>
+      <c r="U41" s="47"/>
+      <c r="V41" s="47"/>
+      <c r="W41" s="47"/>
+      <c r="X41" s="47"/>
+      <c r="Y41" s="47"/>
+      <c r="Z41" s="47"/>
+      <c r="AA41" s="47"/>
+      <c r="AB41" s="47"/>
+      <c r="AC41" s="47"/>
+      <c r="AD41" s="47"/>
+      <c r="AE41" s="47"/>
+      <c r="AF41" s="47"/>
+      <c r="AG41" s="47"/>
+      <c r="AH41" s="48"/>
+    </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
+      <c r="A42" s="8"/>
       <c r="B42" s="46" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C42" s="47"/>
       <c r="D42" s="47"/>
@@ -2449,9 +2403,9 @@
       <c r="AH42" s="48"/>
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C43" s="47"/>
       <c r="D43" s="47"/>
@@ -2487,118 +2441,83 @@
       <c r="AH43" s="48"/>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
-      <c r="B44" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="47"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="47"/>
-      <c r="M44" s="47"/>
-      <c r="N44" s="47"/>
-      <c r="O44" s="47"/>
-      <c r="P44" s="47"/>
-      <c r="Q44" s="47"/>
-      <c r="R44" s="47"/>
-      <c r="S44" s="47"/>
-      <c r="T44" s="47"/>
-      <c r="U44" s="47"/>
-      <c r="V44" s="47"/>
-      <c r="W44" s="47"/>
-      <c r="X44" s="47"/>
-      <c r="Y44" s="47"/>
-      <c r="Z44" s="47"/>
-      <c r="AA44" s="47"/>
-      <c r="AB44" s="47"/>
-      <c r="AC44" s="47"/>
-      <c r="AD44" s="47"/>
-      <c r="AE44" s="47"/>
-      <c r="AF44" s="47"/>
-      <c r="AG44" s="47"/>
-      <c r="AH44" s="48"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="2"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
-      <c r="B45" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="2"/>
-      <c r="Z45" s="2"/>
-      <c r="AA45" s="2"/>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="2"/>
-      <c r="AD45" s="2"/>
-      <c r="AE45" s="2"/>
-      <c r="AF45" s="2"/>
-      <c r="AG45" s="2"/>
-      <c r="AH45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="47"/>
+      <c r="O45" s="47"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="47"/>
+      <c r="R45" s="47"/>
+      <c r="S45" s="47"/>
+      <c r="T45" s="47"/>
+      <c r="U45" s="47"/>
+      <c r="V45" s="47"/>
+      <c r="W45" s="47"/>
+      <c r="X45" s="47"/>
+      <c r="Y45" s="47"/>
+      <c r="Z45" s="47"/>
+      <c r="AA45" s="47"/>
+      <c r="AB45" s="47"/>
+      <c r="AC45" s="47"/>
+      <c r="AD45" s="47"/>
+      <c r="AE45" s="47"/>
+      <c r="AF45" s="47"/>
+      <c r="AG45" s="47"/>
+      <c r="AH45" s="48"/>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="47"/>
-      <c r="M46" s="47"/>
-      <c r="N46" s="47"/>
-      <c r="O46" s="47"/>
-      <c r="P46" s="47"/>
-      <c r="Q46" s="47"/>
-      <c r="R46" s="47"/>
-      <c r="S46" s="47"/>
-      <c r="T46" s="47"/>
-      <c r="U46" s="47"/>
-      <c r="V46" s="47"/>
-      <c r="W46" s="47"/>
-      <c r="X46" s="47"/>
-      <c r="Y46" s="47"/>
-      <c r="Z46" s="47"/>
-      <c r="AA46" s="47"/>
-      <c r="AB46" s="47"/>
-      <c r="AC46" s="47"/>
-      <c r="AD46" s="47"/>
-      <c r="AE46" s="47"/>
-      <c r="AF46" s="47"/>
-      <c r="AG46" s="47"/>
-      <c r="AH46" s="48"/>
+      <c r="A46" s="6"/>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
@@ -5456,14 +5375,11 @@
     <row r="998" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A998" s="6"/>
     </row>
-    <row r="999" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A999" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B42:AH42"/>
     <mergeCell ref="B43:AH43"/>
-    <mergeCell ref="B44:AH44"/>
-    <mergeCell ref="B46:AH46"/>
+    <mergeCell ref="B45:AH45"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
@@ -5471,11 +5387,11 @@
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="AA1:AD1"/>
-    <mergeCell ref="P2:Q36"/>
-    <mergeCell ref="R2:R36"/>
-    <mergeCell ref="AG2:AH36"/>
+    <mergeCell ref="P2:Q35"/>
+    <mergeCell ref="R2:R35"/>
+    <mergeCell ref="AG2:AH35"/>
     <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="B42:AH42"/>
+    <mergeCell ref="B41:AH41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>